<commit_message>
Actualizacion Documento y Excel con el Req 5
</commit_message>
<xml_diff>
--- a/Docs/Reto_3_Graficas.xlsx
+++ b/Docs/Reto_3_Graficas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/s_velasquezm2_uniandes_edu_co/Documents/Documentos/UNIANDES/Segundo Semestre(2021-2)/EDA/Reto 3/Reto3-G02/Docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\Segundo Semestre\Estructura de Datos\Laboratorios\Modulo 3\Reto3-G02\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{A1117D5F-E37C-4EDF-88FA-8CF2B91D82D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CEFBBEE3-0111-4235-A0F6-168B30C0648C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1FCC8D-5031-4C93-91DA-6144C62BA911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="764" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="2445" windowWidth="21600" windowHeight="11295" tabRatio="764" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Graf ARRAYLIST" sheetId="2" state="hidden" r:id="rId1"/>
@@ -410,7 +410,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-MX"/>
   <c:roundedCorners val="1"/>
   <c:style val="2"/>
   <c:chart>
@@ -522,7 +522,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2146822103"/>
@@ -564,7 +564,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -578,7 +578,7 @@
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-MX"/>
   <c:roundedCorners val="1"/>
   <c:style val="2"/>
   <c:chart>
@@ -931,7 +931,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="726611238"/>
@@ -1001,7 +1001,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="196073028"/>
@@ -1024,7 +1024,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1038,7 +1038,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-MX"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1100,7 +1100,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1296,7 +1296,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1334,7 +1334,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="30643311"/>
@@ -1421,7 +1421,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1453,7 +1453,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="30642479"/>
@@ -1495,7 +1495,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1532,7 +1532,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1541,7 +1541,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-MX"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1634,7 +1634,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1830,7 +1830,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1868,7 +1868,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="30493807"/>
@@ -1963,7 +1963,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1995,7 +1995,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="30492975"/>
@@ -2037,7 +2037,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2074,7 +2074,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -2083,7 +2083,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-MX"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2150,7 +2150,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2346,7 +2346,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2384,7 +2384,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="29335439"/>
@@ -2471,7 +2471,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2503,7 +2503,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="29333775"/>
@@ -2549,7 +2549,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2586,7 +2586,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -2595,7 +2595,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-MX"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2662,7 +2662,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2858,7 +2858,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2896,7 +2896,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="39512863"/>
@@ -2983,7 +2983,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3015,7 +3015,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="39510783"/>
@@ -3057,7 +3057,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3094,7 +3094,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -3103,7 +3103,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-MX"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3170,7 +3170,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3256,6 +3256,27 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15.625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.625</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.625</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.625</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.625</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3342,7 +3363,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3380,7 +3401,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1944068239"/>
@@ -3467,7 +3488,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3499,7 +3520,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1944067823"/>
@@ -3541,7 +3562,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3578,7 +3599,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -3587,7 +3608,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-MX"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3624,7 +3645,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4150,6 +4171,30 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.625</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.625</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.625</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.625</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.625</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4236,7 +4281,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4274,7 +4319,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2021141167"/>
@@ -4361,7 +4406,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4393,7 +4438,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2021143663"/>
@@ -4435,7 +4480,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4472,7 +4517,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -4481,7 +4526,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-MX"/>
   <c:roundedCorners val="1"/>
   <c:style val="2"/>
   <c:chart>
@@ -4593,7 +4638,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="302005758"/>
@@ -4635,7 +4680,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4649,7 +4694,7 @@
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-MX"/>
   <c:roundedCorners val="1"/>
   <c:style val="2"/>
   <c:chart>
@@ -4770,7 +4815,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1670929339"/>
@@ -4812,7 +4857,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -8107,7 +8152,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3387E470-FA8F-41A0-82D6-2DC8BF07B9D7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="78" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8118,7 +8163,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3B3F4C8E-60D8-431B-AA06-C84D4B03F68B}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="78" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8129,7 +8174,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{06F7256C-024A-4B47-B9F1-6375612645D3}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="78" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8140,7 +8185,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{CBE35FC9-B63B-41FB-812A-2527D36C06DC}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="78" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8151,7 +8196,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{1DD86D0D-60C6-4CDD-A603-AFD90084E5E3}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="78" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8261,7 +8306,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="13017500" cy="9439519"/>
+    <xdr:ext cx="8663836" cy="6289110"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -8294,7 +8339,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="13023273" cy="9438409"/>
+    <xdr:ext cx="8663836" cy="6289110"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -8327,7 +8372,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="13017500" cy="9439519"/>
+    <xdr:ext cx="8663836" cy="6289110"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -8360,7 +8405,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="13017500" cy="9439519"/>
+    <xdr:ext cx="8663836" cy="6289110"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -8393,7 +8438,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="13017500" cy="9439519"/>
+    <xdr:ext cx="8663836" cy="6289110"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -8426,7 +8471,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="13017500" cy="9439519"/>
+    <xdr:ext cx="8654143" cy="6272893"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -8737,35 +8782,35 @@
   <dimension ref="B1:G67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="40.5" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.875" customWidth="1"/>
     <col min="4" max="4" width="21.5" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.375" customWidth="1"/>
     <col min="6" max="6" width="21.5" customWidth="1"/>
-    <col min="7" max="7" width="18.08203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.125" style="2" customWidth="1"/>
     <col min="8" max="8" width="21.5" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" customWidth="1"/>
+    <col min="9" max="9" width="11.375" customWidth="1"/>
     <col min="10" max="10" width="21.5" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" customWidth="1"/>
+    <col min="11" max="11" width="11.375" customWidth="1"/>
     <col min="12" max="12" width="21.5" customWidth="1"/>
-    <col min="13" max="13" width="11.33203125" customWidth="1"/>
+    <col min="13" max="13" width="11.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.2">
       <c r="G1"/>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="G2"/>
     </row>
-    <row r="3" spans="2:7" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G3"/>
     </row>
-    <row r="4" spans="2:7" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
@@ -8785,7 +8830,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -8801,9 +8846,11 @@
       <c r="F5" s="3">
         <v>0</v>
       </c>
-      <c r="G5" s="3"/>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
         <v>0.05</v>
       </c>
@@ -8819,9 +8866,11 @@
       <c r="F6" s="3">
         <v>15.625</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="3">
+        <v>15.625</v>
+      </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>0.1</v>
       </c>
@@ -8837,9 +8886,11 @@
       <c r="F7" s="3">
         <v>15.625</v>
       </c>
-      <c r="G7" s="3"/>
+      <c r="G7" s="3">
+        <v>15.625</v>
+      </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <v>0.2</v>
       </c>
@@ -8855,9 +8906,11 @@
       <c r="F8" s="3">
         <v>15.625</v>
       </c>
-      <c r="G8" s="3"/>
+      <c r="G8" s="3">
+        <v>15.625</v>
+      </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
         <v>0.3</v>
       </c>
@@ -8873,9 +8926,11 @@
       <c r="F9" s="3">
         <v>15.625</v>
       </c>
-      <c r="G9" s="3"/>
+      <c r="G9" s="3">
+        <v>15.625</v>
+      </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <v>0.5</v>
       </c>
@@ -8891,9 +8946,11 @@
       <c r="F10" s="3">
         <v>15.625</v>
       </c>
-      <c r="G10" s="3"/>
+      <c r="G10" s="3">
+        <v>15.625</v>
+      </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>0.8</v>
       </c>
@@ -8909,9 +8966,11 @@
       <c r="F11" s="3">
         <v>15.625</v>
       </c>
-      <c r="G11" s="3"/>
+      <c r="G11" s="3">
+        <v>15.625</v>
+      </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
         <v>1</v>
       </c>
@@ -8927,290 +8986,292 @@
       <c r="F12" s="3">
         <v>15.625</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="3">
+        <v>15.625</v>
+      </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="G13"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="G14"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="G15"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="G16"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="G17"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="G18"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" s="1"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="G19"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="1"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="G20"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" s="1"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="G21"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" s="1"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="G22"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" s="1"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="G23"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" s="1"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="G24"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B25" s="1"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="G25"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B26" s="1"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="G26"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B27" s="1"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="G27"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B28" s="1"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="G28"/>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B29" s="1"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="G29"/>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B30" s="1"/>
       <c r="C30" s="4"/>
       <c r="D30" s="3"/>
       <c r="G30"/>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B31" s="1"/>
       <c r="C31" s="4"/>
       <c r="D31" s="3"/>
       <c r="G31"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B32" s="1"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="G32"/>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="G33"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B34" s="1"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="G34"/>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="G35"/>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="G36"/>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B37" s="1"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="G37"/>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B38" s="1"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="G38"/>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B39" s="1"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="G39"/>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B40" s="1"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="G40"/>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B41" s="1"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="G41"/>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B42" s="1"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B43" s="1"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B44" s="1"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B45" s="1"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B46" s="1"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B47" s="1"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B48" s="1"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49" s="1"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B50" s="1"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B51" s="1"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B52" s="1"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B53" s="1"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B54" s="1"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B55" s="1"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B56" s="1"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B57" s="1"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B58" s="1"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B59" s="1"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B60" s="1"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B61" s="1"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B62" s="1"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B63" s="1"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B64" s="1"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B65" s="1"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B66" s="1"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B67" s="1"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>

</xml_diff>

<commit_message>
Grafica Req 6 (Bono)
</commit_message>
<xml_diff>
--- a/Docs/Reto_3_Graficas.xlsx
+++ b/Docs/Reto_3_Graficas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\Segundo Semestre\Estructura de Datos\Laboratorios\Modulo 3\Reto3-G02\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/s_velasquezm2_uniandes_edu_co/Documents/Documentos/UNIANDES/Segundo Semestre(2021-2)/EDA/Reto 3/Reto3-G02/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCBA5E0A-4D56-48BB-85E4-2B7DB0DE22EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{BCBA5E0A-4D56-48BB-85E4-2B7DB0DE22EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33EC43A9-076D-4EC2-8757-DA0B7DA90FD4}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="2445" windowWidth="21600" windowHeight="11295" tabRatio="764" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="764" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Graf ARRAYLIST" sheetId="2" state="hidden" r:id="rId1"/>
@@ -20,18 +20,19 @@
     <sheet name="R3" sheetId="33" r:id="rId5"/>
     <sheet name="R4" sheetId="34" r:id="rId6"/>
     <sheet name="R5" sheetId="35" r:id="rId7"/>
-    <sheet name="Req comparacion" sheetId="40" r:id="rId8"/>
-    <sheet name="Gráfico1" sheetId="41" r:id="rId9"/>
-    <sheet name="Graf Insertion Sort" sheetId="3" state="hidden" r:id="rId10"/>
-    <sheet name="Graf LINKED_LIST" sheetId="4" state="hidden" r:id="rId11"/>
-    <sheet name="Graf Shell Sort" sheetId="5" state="hidden" r:id="rId12"/>
+    <sheet name="Bono" sheetId="42" r:id="rId8"/>
+    <sheet name="Req comparacion" sheetId="40" r:id="rId9"/>
+    <sheet name="Gráfico1" sheetId="41" r:id="rId10"/>
+    <sheet name="Graf Insertion Sort" sheetId="3" state="hidden" r:id="rId11"/>
+    <sheet name="Graf LINKED_LIST" sheetId="4" state="hidden" r:id="rId12"/>
+    <sheet name="Graf Shell Sort" sheetId="5" state="hidden" r:id="rId13"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>0,50%</t>
   </si>
@@ -52,6 +53,9 @@
   </si>
   <si>
     <t>Req 5</t>
+  </si>
+  <si>
+    <t>Req 6</t>
   </si>
 </sst>
 </file>
@@ -118,7 +122,26 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -368,28 +391,30 @@
   </dxfs>
   <tableStyles count="4">
     <tableStyle name="Datos Lab4-5-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="19"/>
-      <tableStyleElement type="firstRowStripe" dxfId="18"/>
-      <tableStyleElement type="secondRowStripe" dxfId="17"/>
+      <tableStyleElement type="headerRow" dxfId="20"/>
+      <tableStyleElement type="firstRowStripe" dxfId="19"/>
+      <tableStyleElement type="secondRowStripe" dxfId="18"/>
     </tableStyle>
     <tableStyle name="Datos Lab4-5-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="headerRow" dxfId="16"/>
-      <tableStyleElement type="firstRowStripe" dxfId="15"/>
-      <tableStyleElement type="secondRowStripe" dxfId="14"/>
+      <tableStyleElement type="headerRow" dxfId="17"/>
+      <tableStyleElement type="firstRowStripe" dxfId="16"/>
+      <tableStyleElement type="secondRowStripe" dxfId="15"/>
     </tableStyle>
     <tableStyle name="Datos Lab4-5-style 3" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
-      <tableStyleElement type="headerRow" dxfId="13"/>
-      <tableStyleElement type="firstRowStripe" dxfId="12"/>
-      <tableStyleElement type="secondRowStripe" dxfId="11"/>
+      <tableStyleElement type="headerRow" dxfId="14"/>
+      <tableStyleElement type="firstRowStripe" dxfId="13"/>
+      <tableStyleElement type="secondRowStripe" dxfId="12"/>
     </tableStyle>
     <tableStyle name="Datos Lab4-5-style 4" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF03000000}">
-      <tableStyleElement type="headerRow" dxfId="10"/>
-      <tableStyleElement type="firstRowStripe" dxfId="9"/>
-      <tableStyleElement type="secondRowStripe" dxfId="8"/>
+      <tableStyleElement type="headerRow" dxfId="11"/>
+      <tableStyleElement type="firstRowStripe" dxfId="10"/>
+      <tableStyleElement type="secondRowStripe" dxfId="9"/>
     </tableStyle>
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FFFFFF00"/>
+      <color rgb="FFCC00CC"/>
       <color rgb="FFFF6600"/>
       <color rgb="FFFF0066"/>
       <color rgb="FFCC0099"/>
@@ -411,7 +436,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="1"/>
   <c:style val="2"/>
   <c:chart>
@@ -523,7 +548,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2146822103"/>
@@ -565,7 +590,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -579,7 +604,175 @@
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="1400" b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Comparación de tiempos de ejecucion para Insertion Sort</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1588610115"/>
+        <c:axId val="302005758"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1588610115"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr sz="1000" b="1" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>Tamaño de la muestra [Num. elementos]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="900" b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="302005758"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="302005758"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="1588610115"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr sz="900" b="0" i="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="1"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="1"/>
   <c:style val="2"/>
   <c:chart>
@@ -700,7 +893,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1670929339"/>
@@ -742,7 +935,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -753,10 +946,10 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="1"/>
   <c:style val="2"/>
   <c:chart>
@@ -1109,7 +1302,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="726611238"/>
@@ -1179,7 +1372,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="196073028"/>
@@ -1202,7 +1395,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1216,7 +1409,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1278,7 +1471,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1474,7 +1667,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1512,7 +1705,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="30643311"/>
@@ -1599,7 +1792,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1631,7 +1824,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="30642479"/>
@@ -1673,7 +1866,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1710,7 +1903,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1719,7 +1912,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1812,7 +2005,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2008,7 +2201,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2046,7 +2239,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="30493807"/>
@@ -2141,7 +2334,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2173,7 +2366,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="30492975"/>
@@ -2215,7 +2408,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2252,7 +2445,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -2261,7 +2454,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2328,7 +2521,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2524,7 +2717,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2562,7 +2755,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="29335439"/>
@@ -2649,7 +2842,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2681,7 +2874,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="29333775"/>
@@ -2727,7 +2920,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2764,7 +2957,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -2773,7 +2966,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2840,7 +3033,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3036,7 +3229,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3074,7 +3267,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="39512863"/>
@@ -3161,7 +3354,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3193,7 +3386,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="39510783"/>
@@ -3235,7 +3428,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3272,7 +3465,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -3281,7 +3474,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3348,7 +3541,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3544,7 +3737,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3582,7 +3775,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1944068239"/>
@@ -3669,7 +3862,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3701,7 +3894,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1944067823"/>
@@ -3743,7 +3936,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3780,7 +3973,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -3789,7 +3982,515 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CO" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Requerimiento 6 (Bono)</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-CO">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Tiempo de ejecucion '!$H$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Req 6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Tiempo de ejecucion '!$B$5:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0,50%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5%</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10%</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20%</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30%</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50%</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80%</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Tiempo de ejecucion '!$H$5:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2292-4793-8140-A42F555818D4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1790220799"/>
+        <c:axId val="1790221215"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1790220799"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="0" i="0" cap="all" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Tamaño de la muestra [Num. elementos]</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-CO" sz="1200">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1790221215"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1790221215"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-CO" sz="1200" b="0" i="0" cap="all" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Tiempo de ejecución [ms]</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-CO" sz="1200">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1790220799"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3856,7 +4557,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4413,6 +5114,116 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-A467-40E4-AF60-596267A2CDC4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Tiempo de ejecucion '!$H$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Req 6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Tiempo de ejecucion '!$B$5:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0,50%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5%</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10%</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20%</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30%</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50%</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80%</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Tiempo de ejecucion '!$H$5:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D17E-4D79-A20B-905C7C31B7E9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4492,7 +5303,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4530,7 +5341,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2021141167"/>
@@ -4617,7 +5428,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4649,7 +5460,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2021143663"/>
@@ -4691,7 +5502,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4728,16 +5539,16 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4804,7 +5615,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5359,6 +6170,108 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-D2B9-4BFD-A869-07230BC96835}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Tiempo de ejecucion '!$H$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Req 6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d>
+              <a:contourClr>
+                <a:schemeClr val="accent4"/>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Tiempo de ejecucion '!$B$5:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0,50%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5%</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10%</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20%</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30%</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50%</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80%</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Tiempo de ejecucion '!$H$5:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3C94-4241-B998-5201CB1BF361}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5437,7 +6350,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5475,7 +6388,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1520997536"/>
@@ -5562,7 +6475,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5594,7 +6507,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1560537776"/>
@@ -5719,7 +6632,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5750,7 +6663,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1520997536"/>
@@ -5791,7 +6704,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5828,177 +6741,9 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="1"/>
-  <c:lang val="es-MX"/>
-  <c:roundedCorners val="1"/>
-  <c:style val="2"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr sz="1400" b="0" i="0">
-                <a:solidFill>
-                  <a:srgbClr val="757575"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0">
-                <a:solidFill>
-                  <a:srgbClr val="757575"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:rPr>
-              <a:t>Comparación de tiempos de ejecucion para Insertion Sort</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1588610115"/>
-        <c:axId val="302005758"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1588610115"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr sz="1000" b="1" i="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="1" i="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t>Tamaño de la muestra [Num. elementos]</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr sz="900" b="0" i="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="302005758"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="302005758"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="cross"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="1588610115"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0">
-            <a:defRPr sz="900" b="0" i="0">
-              <a:solidFill>
-                <a:srgbClr val="1A1A1A"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="1"/>
-  </c:chart>
 </c:chartSpace>
 </file>
 
@@ -6282,6 +7027,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -9301,6 +10086,509 @@
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9815,6 +11103,17 @@
 </file>
 
 <file path=xl/chartsheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="55" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr/>
   <sheetViews>
@@ -9825,7 +11124,7 @@
 </chartsheet>
 </file>
 
-<file path=xl/chartsheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/chartsheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr/>
   <sheetViews>
@@ -9840,7 +11139,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3387E470-FA8F-41A0-82D6-2DC8BF07B9D7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="64" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9851,7 +11150,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3B3F4C8E-60D8-431B-AA06-C84D4B03F68B}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="64" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9862,7 +11161,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{06F7256C-024A-4B47-B9F1-6375612645D3}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="64" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9873,7 +11172,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{CBE35FC9-B63B-41FB-812A-2527D36C06DC}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="64" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9884,7 +11183,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{1DD86D0D-60C6-4CDD-A603-AFD90084E5E3}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="78" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="64" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9892,6 +11191,17 @@
 </file>
 
 <file path=xl/chartsheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{ED841C59-2600-46FC-8630-C0DBF8B71405}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="64" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{F6895671-A7DF-4277-A107-D5A78302D4AB}">
   <sheetPr/>
   <sheetViews>
@@ -9902,22 +11212,11 @@
 </chartsheet>
 </file>
 
-<file path=xl/chartsheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/chartsheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{048210E7-8445-497A-9C58-DD385C8154CB}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
-  </sheetViews>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</chartsheet>
-</file>
-
-<file path=xl/chartsheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr/>
-  <sheetViews>
-    <sheetView zoomScale="55" workbookViewId="0"/>
+    <sheetView zoomScale="64" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9961,6 +11260,39 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="13005955" cy="9438409"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
     <xdr:ext cx="12992100" cy="9429750"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9990,7 +11322,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -10027,7 +11359,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8663836" cy="6289110"/>
+    <xdr:ext cx="8661797" cy="6290469"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -10060,7 +11392,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8663836" cy="6289110"/>
+    <xdr:ext cx="8661797" cy="6290469"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -10093,7 +11425,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8663836" cy="6289110"/>
+    <xdr:ext cx="8661797" cy="6290469"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -10126,7 +11458,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8663836" cy="6289110"/>
+    <xdr:ext cx="8661797" cy="6290469"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -10159,7 +11491,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="13017500" cy="9439519"/>
+    <xdr:ext cx="8661797" cy="6290469"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -10192,7 +11524,40 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="12994821" cy="9416143"/>
+    <xdr:ext cx="8661797" cy="6290469"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7A9440F-C85A-43A7-BF5E-8D9A0ABBF150}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8654143" cy="6277429"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -10221,11 +11586,11 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8663836" cy="6289110"/>
+    <xdr:ext cx="8661797" cy="6290469"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -10254,49 +11619,17 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:absoluteAnchor>
-    <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="13005955" cy="9438409"/>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:absoluteAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9AEAAB3A-C3B6-4DA8-A862-2C4181B2A2D0}" name="Tabla6" displayName="Tabla6" ref="B4:G12" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B4:G12" xr:uid="{9AEAAB3A-C3B6-4DA8-A862-2C4181B2A2D0}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{35F8E59E-F7B0-4AC4-BD4B-D21E3BE3A01F}" name="Tamaño de la muestra [Num. Elementos]" dataDxfId="5" dataCellStyle="Porcentaje"/>
-    <tableColumn id="2" xr3:uid="{C9D433A3-2FD1-42A8-A5AD-8037A2DA2580}" name="Req 1" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{8C8A79AC-1016-4750-9155-0B7FD7285FB0}" name="Req 2" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{67B8A5A9-6ABE-4B94-AD38-D5C5E9125162}" name="Req 3" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{9BF81073-AF23-459C-9DEE-218A28F495FD}" name="Req 4" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{7518681F-7EF8-4811-9585-A5092816CC35}" name="Req 5" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9AEAAB3A-C3B6-4DA8-A862-2C4181B2A2D0}" name="Tabla6" displayName="Tabla6" ref="B4:H12" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="B4:H12" xr:uid="{9AEAAB3A-C3B6-4DA8-A862-2C4181B2A2D0}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{35F8E59E-F7B0-4AC4-BD4B-D21E3BE3A01F}" name="Tamaño de la muestra [Num. Elementos]" dataDxfId="6" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" xr3:uid="{C9D433A3-2FD1-42A8-A5AD-8037A2DA2580}" name="Req 1" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{8C8A79AC-1016-4750-9155-0B7FD7285FB0}" name="Req 2" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{67B8A5A9-6ABE-4B94-AD38-D5C5E9125162}" name="Req 3" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{9BF81073-AF23-459C-9DEE-218A28F495FD}" name="Req 4" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{7518681F-7EF8-4811-9585-A5092816CC35}" name="Req 5" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{5C46FBFB-5208-4565-87B0-47D61E814800}" name="Req 6" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10500,38 +11833,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{427B42F3-5FE2-4A71-B278-3B07F783DD93}">
-  <dimension ref="B1:G67"/>
+  <dimension ref="B1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="40.5" customWidth="1"/>
-    <col min="3" max="3" width="18.875" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
     <col min="4" max="4" width="21.5" customWidth="1"/>
-    <col min="5" max="5" width="19.375" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
     <col min="6" max="6" width="21.5" customWidth="1"/>
-    <col min="7" max="7" width="18.125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.08203125" style="2" customWidth="1"/>
     <col min="8" max="8" width="21.5" customWidth="1"/>
-    <col min="9" max="9" width="11.375" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
     <col min="10" max="10" width="21.5" customWidth="1"/>
-    <col min="11" max="11" width="11.375" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" customWidth="1"/>
     <col min="12" max="12" width="21.5" customWidth="1"/>
-    <col min="13" max="13" width="11.375" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
       <c r="G1"/>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="G2"/>
     </row>
-    <row r="3" spans="2:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:8" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G3"/>
     </row>
-    <row r="4" spans="2:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:8" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
@@ -10550,8 +11883,11 @@
       <c r="G4" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="H4" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -10570,8 +11906,11 @@
       <c r="G5" s="3">
         <v>0</v>
       </c>
+      <c r="H5" s="3">
+        <v>125</v>
+      </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>0.05</v>
       </c>
@@ -10590,8 +11929,11 @@
       <c r="G6" s="3">
         <v>15.625</v>
       </c>
+      <c r="H6" s="3">
+        <v>125</v>
+      </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>0.1</v>
       </c>
@@ -10610,8 +11952,11 @@
       <c r="G7" s="3">
         <v>15.625</v>
       </c>
+      <c r="H7" s="3">
+        <v>125</v>
+      </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>0.2</v>
       </c>
@@ -10630,8 +11975,11 @@
       <c r="G8" s="3">
         <v>15.625</v>
       </c>
+      <c r="H8" s="3">
+        <v>125</v>
+      </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>0.3</v>
       </c>
@@ -10650,8 +11998,11 @@
       <c r="G9" s="3">
         <v>15.625</v>
       </c>
+      <c r="H9" s="3">
+        <v>125</v>
+      </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>0.5</v>
       </c>
@@ -10670,8 +12021,11 @@
       <c r="G10" s="3">
         <v>15.625</v>
       </c>
+      <c r="H10" s="3">
+        <v>125</v>
+      </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <v>0.8</v>
       </c>
@@ -10690,8 +12044,11 @@
       <c r="G11" s="3">
         <v>15.625</v>
       </c>
+      <c r="H11" s="3">
+        <v>125</v>
+      </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
         <v>1</v>
       </c>
@@ -10710,289 +12067,292 @@
       <c r="G12" s="3">
         <v>15.625</v>
       </c>
+      <c r="H12" s="3">
+        <v>125</v>
+      </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="G13"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="G14"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="G15"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="G16"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="G17"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="G18"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="G19"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="G20"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="G21"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="G22"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="G23"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="G24"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="G25"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="G26"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="G27"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="G28"/>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="G29"/>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
       <c r="C30" s="4"/>
       <c r="D30" s="3"/>
       <c r="G30"/>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
       <c r="C31" s="4"/>
       <c r="D31" s="3"/>
       <c r="G31"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="G32"/>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="G33"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="G34"/>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="G35"/>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="G36"/>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B37" s="1"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="G37"/>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="G38"/>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="G39"/>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B40" s="1"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="G40"/>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="G41"/>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B44" s="1"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B45" s="1"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B46" s="1"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B47" s="1"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B48" s="1"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49" s="1"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" s="1"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51" s="1"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B52" s="1"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B53" s="1"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B54" s="1"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B55" s="1"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B56" s="1"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B57" s="1"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B58" s="1"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B59" s="1"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B60" s="1"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B61" s="1"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B62" s="1"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B63" s="1"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B64" s="1"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B65" s="1"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B66" s="1"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B67" s="1"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>

</xml_diff>